<commit_message>
exclude trade + fixed powerDemand
</commit_message>
<xml_diff>
--- a/opperational_costs_2019_2.xlsx
+++ b/opperational_costs_2019_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\SpiderOak Hive\Uni\epm\project\epmProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\CloudDrive\Uni\SS24\CaseStudies\gamsFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9C26A1-CD7D-4D67-A90A-D62B53C05289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C8E46F-B0CC-4BF8-B121-E9F5659EDAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -465,15 +465,15 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -489,7 +489,7 @@
         <v>31.222214461095714</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -497,7 +497,7 @@
         <v>66.589869760375592</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -505,7 +505,7 @@
         <v>27.462599999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -513,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -529,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -537,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -545,7 +545,7 @@
         <v>17.866666666666664</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -561,7 +561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -569,7 +569,7 @@
         <v>9.861600880825014</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -577,7 +577,7 @@
         <v>94.799925554493257</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -585,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -593,7 +593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -601,7 +601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>

</xml_diff>